<commit_message>
Add the entire framework of calculations
</commit_message>
<xml_diff>
--- a/code/meat_RR_2019.xlsx
+++ b/code/meat_RR_2019.xlsx
@@ -566,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1811,7 +1811,7 @@
         <v>1.1599999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="48" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:19" ht="24" x14ac:dyDescent="0.75">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
@@ -2047,7 +2047,7 @@
         <v>1.1599999999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="48" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:19" ht="24" x14ac:dyDescent="0.75">
       <c r="A26" s="1" t="s">
         <v>6</v>
       </c>
@@ -2165,7 +2165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="48" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:19" ht="24" x14ac:dyDescent="0.75">
       <c r="A28" s="1" t="s">
         <v>7</v>
       </c>

</xml_diff>